<commit_message>
start wavelet analysis of summary statistics
</commit_message>
<xml_diff>
--- a/observations_depthlogs_migration_residency.xlsx
+++ b/observations_depthlogs_migration_residency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lotte.pohl\Documents\github_repos\MasterThesis_LottePohl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F45255ED-C1CE-4F74-9D26-986CEBD22677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919549F3-1944-4A4F-8E0A-21BD43A8A045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C64583E7-21D2-4ACD-A991-7201B20D2126}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>tag_nr</t>
   </si>
@@ -72,6 +72,33 @@
   </si>
   <si>
     <t>sr</t>
+  </si>
+  <si>
+    <t>sm</t>
+  </si>
+  <si>
+    <t>median depth change</t>
+  </si>
+  <si>
+    <t>sum of change of median depth per week is &lt;&lt; 0</t>
+  </si>
+  <si>
+    <t>sum of absolute change of median depth per week &gt;&gt;0</t>
+  </si>
+  <si>
+    <t>sum of change of median depth per week == 0</t>
+  </si>
+  <si>
+    <t>mean change of median depth per week == 0</t>
+  </si>
+  <si>
+    <t>sd of change of median depth per week &gt;&gt; 0</t>
+  </si>
+  <si>
+    <t>sd of change of median depth per week == 0</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -432,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A720E78E-D057-4D99-93ED-6DD16DE24848}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,6 +541,176 @@
         <v>6</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>321</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
+        <v>321</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>321</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>321</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>321</v>
+      </c>
+      <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>321</v>
+      </c>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>308</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>308</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>308</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>308</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update thesis manuscript and .gitignore
</commit_message>
<xml_diff>
--- a/observations_depthlogs_migration_residency.xlsx
+++ b/observations_depthlogs_migration_residency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lotte.pohl\Documents\github_repos\MasterThesis_LottePohl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919549F3-1944-4A4F-8E0A-21BD43A8A045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235FA2BA-E440-424C-9E39-4E1983C0C5E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C64583E7-21D2-4ACD-A991-7201B20D2126}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="38">
   <si>
     <t>tag_nr</t>
   </si>
@@ -99,6 +99,57 @@
   </si>
   <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>wm and sm</t>
+  </si>
+  <si>
+    <t>median depth wavelet</t>
+  </si>
+  <si>
+    <t>high period frequencies in periods between 2 - 10 days</t>
+  </si>
+  <si>
+    <t>low period frequencies in periods between 2 - 15 days</t>
+  </si>
+  <si>
+    <t>high period frequencies in periods either around 2 days or 32 days</t>
+  </si>
+  <si>
+    <t>high period frequencies in periods between 2 and 15 days AND low frequencies around 64 and 128 days</t>
+  </si>
+  <si>
+    <t>depth range wavelet</t>
+  </si>
+  <si>
+    <t>significant high frequencies &gt; 15 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">have  7-10 day rolling window </t>
+  </si>
+  <si>
+    <t>significant high frequencies between 3 and 8 days</t>
+  </si>
+  <si>
+    <t>significant high frequencies between 8 and 16 days</t>
+  </si>
+  <si>
+    <t>significant high frequencies between 2 and 17 days</t>
+  </si>
+  <si>
+    <t>maybe also have a 30-50 days window to look at longer periods, for the residency? Eg depth median change/day wavelet has a significant bereich over ~100 days</t>
+  </si>
+  <si>
+    <t>low period frequencies in periods between 2 - 15 days (yellow)</t>
+  </si>
+  <si>
+    <t>low period frequencies in periods between 2 - 15 days (dark blue)</t>
+  </si>
+  <si>
+    <t>median depth change wavelet (roll3)</t>
+  </si>
+  <si>
+    <t>low period frequencies in periods between 2 - 15 days (blue-green)</t>
   </si>
 </sst>
 </file>
@@ -459,74 +510,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A720E78E-D057-4D99-93ED-6DD16DE24848}">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="18.6328125" customWidth="1"/>
+    <col min="1" max="1" width="28.08984375" customWidth="1"/>
+    <col min="2" max="2" width="18.6328125" customWidth="1"/>
     <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.36328125" customWidth="1"/>
+    <col min="4" max="4" width="31.26953125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>321</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>321</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -538,12 +566,12 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
@@ -552,15 +580,15 @@
         <v>321</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
@@ -569,15 +597,15 @@
         <v>321</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -589,12 +617,12 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -606,12 +634,12 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
@@ -623,7 +651,7 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
@@ -640,24 +668,24 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C11">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
@@ -665,21 +693,21 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C12">
-        <v>308</v>
+        <v>321</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -688,15 +716,15 @@
         <v>308</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>
@@ -708,7 +736,245 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15">
+        <v>308</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>308</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>321</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>321</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>321</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>321</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>321</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>308</v>
+      </c>
+      <c r="D22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>308</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>308</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25">
+        <v>308</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>308</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27">
+        <v>308</v>
+      </c>
+      <c r="D27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>308</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>